<commit_message>
Ajout de la fonctionnalité de scan de QR codes pour la recherche et la gestion des produits dans l'application de gestion de stock. Mise à jour du Dockerfile et des dépendances nécessaires, ainsi que des fichiers d'inventaire et d'historique.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,6 +615,32 @@
         <v>90</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-05-22 12:36:01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Tournevis cruciforme</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>103</v>
+      </c>
+      <c r="F8" t="n">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout des colonnes Stock_Min et Stock_Max dans les données initiales, mise à jour de la fonction de chargement pour gérer ces colonnes, et amélioration des fonctionnalités de recherche et de gestion des alertes de stock. Intégration de la vérification des alertes de stock dans l'interface utilisateur avec des indicateurs visuels. Mise à jour des fichiers d'inventaire et d'historique.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,19 +456,19 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Quantite_Avant</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Quantite_Apres</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantite_Avant</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-22 11:05:34</t>
+          <t>2025-05-23 06:40:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -478,26 +478,28 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Entrée</t>
+          <t>Sortie</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>93</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>103</v>
+      </c>
+      <c r="F2" t="n">
+        <v>102</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-05-22 11:07:13</t>
+          <t>2025-05-23 07:10:26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Vis 6x50mm</t>
+          <t>Clé à molette</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -506,72 +508,76 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>988</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="F3" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-05-22 11:07:32</t>
+          <t>2025-05-23 07:34:03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vis 6x50mm</t>
+          <t>Perceuse sans fil</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Entrée</t>
+          <t>Sortie</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>991</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-05-22 11:12:03</t>
+          <t>2025-05-23 07:34:21</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tournevis cruciforme</t>
+          <t>Perceuse sans fil</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sortie</t>
+          <t>Entrée</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>94</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-05-22 11:15:14</t>
+          <t>2025-05-23 07:34:51</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tournevis cruciforme</t>
+          <t>Perceuse sans fil</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -583,47 +589,47 @@
         <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>92</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-05-22 11:18:07</t>
+          <t>2025-05-23 07:36:07</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tournevis cruciforme</t>
+          <t>Vis 6x50mm</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Entrée</t>
+          <t>Sortie</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>500</v>
       </c>
       <c r="E7" t="n">
-        <v>98</v>
+        <v>991</v>
       </c>
       <c r="F7" t="n">
-        <v>90</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-05-22 12:36:01</t>
+          <t>2025-05-23 07:36:29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tournevis cruciforme</t>
+          <t>Vis 6x50mm</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -632,13 +638,221 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>103</v>
+        <v>491</v>
       </c>
       <c r="F8" t="n">
-        <v>98</v>
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:37:13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Vis 6x50mm</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>503</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:37:45</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Vis 6x50mm</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1503</v>
+      </c>
+      <c r="F10" t="n">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:40:59</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Clé à molette</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="n">
+        <v>23</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:53:38</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Clé à molette</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>23</v>
+      </c>
+      <c r="E12" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:53:53</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Clé à molette</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
+      <c r="E13" t="n">
+        <v>34</v>
+      </c>
+      <c r="F13" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:53:59</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Clé à molette</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>42</v>
+      </c>
+      <c r="F14" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:54:04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Clé à molette</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>45</v>
+      </c>
+      <c r="F15" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:54:14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Clé à molette</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>46</v>
+      </c>
+      <c r="F16" t="n">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification de l'interface utilisateur pour renommer l'action "Voir l'inventaire" en "Magasin" et mise à jour de l'affichage des données de stock. Ajout d'une colonne pour la valeur totale du stock et réorganisation des colonnes dans le tableau. Mise à jour des fichiers d'inventaire et d'historique.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,58 @@
         <v>42</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-23 07:59:24</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Perceuse sans fil</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>6</v>
+      </c>
+      <c r="E17" t="n">
+        <v>9</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-23 08:09:59</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Perceuse sans fil</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>8</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" t="n">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout de la fonctionnalité de demande de matériel, permettant aux utilisateurs de soumettre des demandes via un formulaire. Implémentation de la gestion des demandes avec des options pour approuver, refuser ou mettre en attente les demandes. Mise à jour des fichiers d'historique et d'inventaire pour refléter ces changements.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,6 +907,110 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-23 08:42:06</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Parclose</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Sortie - Demande 20250523_082712</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>9</v>
+      </c>
+      <c r="F19" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-23 08:42:06</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Vis 6x50mm</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sortie - Demande 20250523_082712</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-23 08:42:06</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Tournevis cruciforme</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sortie - Demande 20250523_082712</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>30</v>
+      </c>
+      <c r="F21" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-23 08:42:06</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Marteau 500g</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Sortie - Demande 20250523_082712</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>30</v>
+      </c>
+      <c r="F22" t="n">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout d'une fonction pour retourner l'icône appropriée selon le statut des demandes. Mise à jour de l'affichage des demandes pour inclure des icônes et des couleurs correspondant aux statuts (En attente, Approuvée, Refusée). Amélioration de l'interface utilisateur pour une meilleure visualisation des statuts.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1037,6 +1037,58 @@
         <v>6</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-23 11:20:31</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Tournevis cruciforme</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>29</v>
+      </c>
+      <c r="F24" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-23 11:21:07</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Tournevis cruciforme</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>31</v>
+      </c>
+      <c r="F25" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout de la gestion des emplacements avec des fonctions pour charger, créer, sauvegarder et mettre à jour les informations des emplacements. Amélioration de l'interface utilisateur avec des onglets pour afficher, ajouter et modifier des emplacements, ainsi que des statistiques détaillées. Mise à jour de la configuration de la page pour un affichage en mode large.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1028,6 +1028,223 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:20:15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Import - Nouveau produit</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>25</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>25</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:21:35</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25</v>
+      </c>
+      <c r="F21" t="n">
+        <v>17</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:21:51</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>25</v>
+      </c>
+      <c r="E22" t="n">
+        <v>17</v>
+      </c>
+      <c r="F22" t="n">
+        <v>42</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:22:02</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>42</v>
+      </c>
+      <c r="F23" t="n">
+        <v>34</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:22:07</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>34</v>
+      </c>
+      <c r="F24" t="n">
+        <v>29</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:22:16</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Entrée</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="n">
+        <v>29</v>
+      </c>
+      <c r="F25" t="n">
+        <v>52</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-05-28 07:22:24</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>uuuuuuuuuuu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Sortie</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>52</v>
+      </c>
+      <c r="F26" t="n">
+        <v>40</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2481023879</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changement de l'action "Inventaire" en "Régule" dans l'interface utilisateur et mise à jour des références associées. Modifications des fichiers Excel 'historique.xlsx', 'inventaire_avec_references.xlsx' et 'inventaire_sauvegarde.xlsx' pour refléter ces changements.
</commit_message>
<xml_diff>
--- a/data/historique.xlsx
+++ b/data/historique.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1214,6 +1214,37 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-06-02 08:37:32</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Verrouilleur 600mm 1E 255281</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Régule</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>158</v>
+      </c>
+      <c r="F26" t="n">
+        <v>157</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>6755773992</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>